<commit_message>
updated with pivot table
</commit_message>
<xml_diff>
--- a/content/section4/1.2-navigate/1212.xlsx
+++ b/content/section4/1.2-navigate/1212.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20369"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dave\Dropbox\Ann Murphy Projects\MOS Projects\MO-200 Excel Associate\MO 200 TIY Exercises and Resources\1212\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\kaushalya\consultancy\surana\2025\excel\workshop\content\section4\1.2-navigate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{30FF3A0E-44A8-4864-BFE4-12019894C209}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0305F7-0E14-454D-A0DB-9602B7AA21D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="9870" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Marketing Plan Budget" sheetId="1" r:id="rId1"/>
     <sheet name="Maintenance Schedule" sheetId="2" r:id="rId2"/>
-    <sheet name="Profit Forecast" sheetId="9" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="10" r:id="rId3"/>
+    <sheet name="Profit Forecast" sheetId="9" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="Advances">#REF!</definedName>
@@ -29,6 +30,15 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -60,7 +70,8 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Dave's comment</t>
+My comment
+</t>
         </r>
       </text>
     </comment>
@@ -185,10 +196,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="47">
-  <si>
-    <t>Television Advertising</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="53">
   <si>
     <t>Radio</t>
   </si>
@@ -196,9 +204,6 @@
     <t>Internet</t>
   </si>
   <si>
-    <t>Newspaper Advertising</t>
-  </si>
-  <si>
     <t>New Brand Launch Parties</t>
   </si>
   <si>
@@ -326,6 +331,30 @@
   </si>
   <si>
     <t>Staff HIRE</t>
+  </si>
+  <si>
+    <t>Number of occurencess</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Television marketing</t>
+  </si>
+  <si>
+    <t>Newspaper marketing</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>Q5</t>
   </si>
 </sst>
 </file>
@@ -623,7 +652,7 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="1" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -642,7 +671,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2217,7 +2245,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>726201</xdr:colOff>
+      <xdr:colOff>607218</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>161387</xdr:rowOff>
     </xdr:to>
@@ -2598,41 +2626,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="179" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="24.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="8" width="11.5703125" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="24.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" customWidth="1"/>
+    <col min="4" max="5" width="11.5546875" customWidth="1"/>
+    <col min="6" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" customWidth="1"/>
+    <col min="11" max="11" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="22" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="22" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="J2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3">
         <v>2017</v>
@@ -2653,9 +2683,9 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="B4" s="1">
         <v>21000</v>
@@ -2676,9 +2706,9 @@
         <v>65000</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" s="9">
         <v>7600</v>
@@ -2699,9 +2729,9 @@
         <v>17000</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" s="1">
         <v>12987</v>
@@ -2721,11 +2751,10 @@
       <c r="G6" s="1">
         <v>23000</v>
       </c>
-      <c r="I6" s="14"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="B7" s="1">
         <v>1000</v>
@@ -2745,11 +2774,10 @@
       <c r="G7" s="1">
         <v>10000</v>
       </c>
-      <c r="I7" s="14"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B8" s="1">
         <v>20000</v>
@@ -2769,11 +2797,10 @@
       <c r="G8" s="1">
         <v>36000</v>
       </c>
-      <c r="I8" s="14"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B9" s="1">
         <v>98000</v>
@@ -2794,9 +2821,9 @@
         <v>170000</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B10" s="1">
         <v>56000</v>
@@ -2816,11 +2843,10 @@
       <c r="G10" s="1">
         <v>90000</v>
       </c>
-      <c r="I10" s="14"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B11" s="12">
         <f>SUM(B4:B10)</f>
@@ -2847,14 +2873,14 @@
         <v>411000</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="O12" s="10"/>
     </row>
-    <row r="31" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D31" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="E31" s="15"/>
+    <row r="31" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D31" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2878,7 +2904,7 @@
     <oddFooter>&amp;L&amp;P of &amp;N &amp;D&amp;D &amp;T&amp;C&amp;Z&amp;F &amp;F &amp;A</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B11:G11" formulaRange="1"/>
+    <ignoredError sqref="B11:F11" formulaRange="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
@@ -2890,287 +2916,287 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H8:I11"/>
+    <sheetView zoomScale="140" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" customWidth="1"/>
     <col min="16" max="16" width="20" bestFit="1" customWidth="1"/>
-    <col min="20" max="25" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="25" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B1" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="P1" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B1" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="P1" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Q2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="R2" s="2" t="s">
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -3193,34 +3219,94 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CAA4ABD-9F58-423C-AAA2-A21C0922FC40}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="24.28515625" customWidth="1"/>
-    <col min="3" max="7" width="11.5703125" customWidth="1"/>
-    <col min="12" max="13" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="24.33203125" customWidth="1"/>
+    <col min="3" max="7" width="11.5546875" customWidth="1"/>
+    <col min="12" max="13" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3">
         <v>2017</v>
@@ -3241,9 +3327,9 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B4" s="8">
         <v>324</v>
@@ -3264,9 +3350,9 @@
         <v>634</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B5" s="8">
         <v>15</v>
@@ -3287,9 +3373,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B6" s="8">
         <v>32</v>
@@ -3310,9 +3396,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B7" s="8">
         <v>111</v>
@@ -3333,9 +3419,9 @@
         <v>210</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B8" s="8">
         <v>2</v>
@@ -3356,9 +3442,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B9" s="8">
         <v>5</v>
@@ -3379,9 +3465,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B10" s="8">
         <v>6</v>
@@ -3402,9 +3488,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B11" s="8">
         <f>SUM(B4:B10)</f>
@@ -3431,11 +3517,11 @@
         <v>987</v>
       </c>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C38" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D38" s="15"/>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C38" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>